<commit_message>
RelatorioBT - 100% automatizado.
</commit_message>
<xml_diff>
--- a/RelatorioBT/ContatosGEST.xlsx
+++ b/RelatorioBT/ContatosGEST.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adtsa\PycharmProjects\RelatorioBT\RelatorioBT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7C19755-A997-41FA-9606-4FF85ADE73C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F901560-D84B-4A96-B184-118556E7C211}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45" yWindow="885" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="1230" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>contato</t>
   </si>
@@ -33,25 +33,7 @@
     <t>msg</t>
   </si>
   <si>
-    <t>Luis</t>
-  </si>
-  <si>
     <t>Lucas</t>
-  </si>
-  <si>
-    <t>Bruno</t>
-  </si>
-  <si>
-    <t>Maria Helena</t>
-  </si>
-  <si>
-    <t>Bruninho</t>
-  </si>
-  <si>
-    <t>João</t>
-  </si>
-  <si>
-    <t>Marcelo</t>
   </si>
 </sst>
 </file>
@@ -369,10 +351,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -391,37 +373,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>